<commit_message>
Update vintages: add surveys, consumption, and investment.
</commit_message>
<xml_diff>
--- a/data/data_monthly/variables_definitions.xlsx
+++ b/data/data_monthly/variables_definitions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Userhome\mokuneva\nowcasting_with_text\hard_data\data_monthly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Userhome\mokuneva\nowcasting_with_text\data\data_monthly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D24E42A-8BE7-426F-A61A-F95B544B002F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BE9C05-8D9C-466E-ACFC-8884CA2385D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>Mnemonic</t>
   </si>
@@ -211,6 +211,57 @@
   </si>
   <si>
     <t>Yields on public debt securities</t>
+  </si>
+  <si>
+    <t>ifo: industry and trade, climate</t>
+  </si>
+  <si>
+    <t>ifoIndTradeClimate</t>
+  </si>
+  <si>
+    <t>Surveys</t>
+  </si>
+  <si>
+    <t>ifo: industry and trade, current situation</t>
+  </si>
+  <si>
+    <t>ifoIndTradeCurrent</t>
+  </si>
+  <si>
+    <t>ifo: industry and trade, expectations</t>
+  </si>
+  <si>
+    <t>ifoIndTradeExp</t>
+  </si>
+  <si>
+    <t>GfK: business cycle expectations</t>
+  </si>
+  <si>
+    <t>GfKBCE</t>
+  </si>
+  <si>
+    <t>GfK: income expectations</t>
+  </si>
+  <si>
+    <t>GfKIE</t>
+  </si>
+  <si>
+    <t>GfK: willigness-to-buy</t>
+  </si>
+  <si>
+    <t>GfKWtB</t>
+  </si>
+  <si>
+    <t>GfK: consumer climate indicator</t>
+  </si>
+  <si>
+    <t>GfKCCI</t>
+  </si>
+  <si>
+    <t>ESI</t>
+  </si>
+  <si>
+    <t>Economics Sentiment Indicator</t>
   </si>
 </sst>
 </file>
@@ -528,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,6 +906,94 @@
         <v>43</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>